<commit_message>
start placing two masters into db. Unique key added to project table. import_project_to_master_db some additional code so project id recorded only once
</commit_message>
<xml_diff>
--- a/tests/resources/milestones_test_master_4_2019.xlsx
+++ b/tests/resources/milestones_test_master_4_2019.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="69">
   <si>
     <t xml:space="preserve">Project/Programme Name</t>
   </si>
@@ -59,6 +59,24 @@
   </si>
   <si>
     <t xml:space="preserve">DFT ID Number</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D5</t>
   </si>
   <si>
     <t xml:space="preserve">Approval MM1</t>
@@ -244,15 +262,16 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <color rgb="FFFC2525"/>
+      <name val="Cambria"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFC2525"/>
-      <name val="Cambria"/>
-      <family val="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -298,12 +317,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -401,7 +424,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="J17" activeCellId="0" sqref="J17"/>
+      <selection pane="bottomLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -463,74 +486,74 @@
       <c r="A3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="D3" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="E3" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="F3" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="G3" s="1" t="n">
-        <v>6</v>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>1</v>
@@ -542,31 +565,31 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="4" t="n">
+        <v>30</v>
+      </c>
+      <c r="B7" s="5" t="n">
         <v>43900</v>
       </c>
       <c r="D7" s="3"/>
-      <c r="F7" s="4" t="n">
+      <c r="F7" s="5" t="n">
         <v>42305</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="4" t="n">
+        <v>31</v>
+      </c>
+      <c r="B8" s="5" t="n">
         <v>43900</v>
       </c>
       <c r="D8" s="3"/>
-      <c r="F8" s="4" t="n">
+      <c r="F8" s="5" t="n">
         <v>42305</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>0</v>
@@ -578,130 +601,130 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D10" s="3"/>
       <c r="F10" s="1" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="4" t="n">
+        <v>49</v>
+      </c>
+      <c r="B14" s="5" t="n">
         <v>44095</v>
       </c>
-      <c r="C14" s="4" t="n">
+      <c r="C14" s="5" t="n">
         <v>41537</v>
       </c>
       <c r="D14" s="3"/>
-      <c r="E14" s="4" t="n">
+      <c r="E14" s="5" t="n">
         <v>39081</v>
       </c>
-      <c r="F14" s="4" t="n">
+      <c r="F14" s="5" t="n">
         <v>41942</v>
       </c>
-      <c r="G14" s="4" t="n">
+      <c r="G14" s="5" t="n">
         <v>42308</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B15" s="4" t="n">
+        <v>50</v>
+      </c>
+      <c r="B15" s="5" t="n">
         <v>44095</v>
       </c>
-      <c r="C15" s="4" t="n">
+      <c r="C15" s="5" t="n">
         <v>41537</v>
       </c>
       <c r="D15" s="3"/>
-      <c r="E15" s="4" t="n">
+      <c r="E15" s="5" t="n">
         <v>39081</v>
       </c>
-      <c r="F15" s="4" t="n">
+      <c r="F15" s="5" t="n">
         <v>41942</v>
       </c>
-      <c r="G15" s="4" t="n">
+      <c r="G15" s="5" t="n">
         <v>42308</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="B16" s="1" t="n">
         <v>0</v>
@@ -722,139 +745,139 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D17" s="3"/>
       <c r="E17" s="1" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>52</v>
+        <v>58</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="1" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B21" s="4" t="n">
+        <v>63</v>
+      </c>
+      <c r="B21" s="5" t="n">
         <v>43815</v>
       </c>
-      <c r="C21" s="4" t="n">
+      <c r="C21" s="5" t="n">
         <v>41153</v>
       </c>
       <c r="D21" s="3"/>
-      <c r="E21" s="4" t="n">
+      <c r="E21" s="5" t="n">
         <v>38504</v>
       </c>
-      <c r="F21" s="4" t="n">
+      <c r="F21" s="5" t="n">
         <v>41789</v>
       </c>
-      <c r="G21" s="4" t="n">
+      <c r="G21" s="5" t="n">
         <v>41106</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B22" s="4" t="n">
+        <v>64</v>
+      </c>
+      <c r="B22" s="5" t="n">
         <v>43815</v>
       </c>
-      <c r="C22" s="4" t="n">
+      <c r="C22" s="5" t="n">
         <v>41153</v>
       </c>
-      <c r="D22" s="4" t="n">
+      <c r="D22" s="5" t="n">
         <v>41548</v>
       </c>
-      <c r="E22" s="4" t="n">
+      <c r="E22" s="5" t="n">
         <v>38504</v>
       </c>
-      <c r="F22" s="4" t="n">
+      <c r="F22" s="5" t="n">
         <v>41789</v>
       </c>
-      <c r="G22" s="4" t="n">
+      <c r="G22" s="5" t="n">
         <v>41106</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B23" s="1" t="n">
         <v>0</v>
@@ -875,46 +898,46 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="1" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
all tests passing. kwargs now at VfMData class level. VfMData class now processes options embedded in kwargs. quarters_list added to Master class.
</commit_message>
<xml_diff>
--- a/tests/resources/milestones_test_master_4_2019.xlsx
+++ b/tests/resources/milestones_test_master_4_2019.xlsx
@@ -46,7 +46,7 @@
     <t xml:space="preserve">DfT Group</t>
   </si>
   <si>
-    <t xml:space="preserve">Aviation</t>
+    <t xml:space="preserve">AMIS</t>
   </si>
   <si>
     <t xml:space="preserve">Roads Places and Environment Group</t>
@@ -509,9 +509,9 @@
   <dimension ref="A1:G1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="63" zoomScaleNormal="63" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="K35" activeCellId="0" sqref="K35"/>
+      <selection pane="bottomLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.5859375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>